<commit_message>
add remove_data function to filter results based on status code and remarks
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Database Column</t>
   </si>
@@ -113,6 +113,18 @@
   </si>
   <si>
     <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debtor.product_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">placement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debtor.card_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_no</t>
   </si>
 </sst>
 </file>
@@ -127,6 +139,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,6 +160,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -191,12 +205,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,144 +341,160 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add FTP connection functionality and update sample data
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SBC CARDS RECOV L1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="FUSE" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t xml:space="preserve">Database Column</t>
   </si>
@@ -343,7 +344,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -506,4 +507,176 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add phone number formatting and validation functions; enhance FTP connection logging
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SBC CARDS RECOV L1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="FUSE" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="GLOBE WIRELESS" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
   <si>
     <t xml:space="preserve">Database Column</t>
   </si>
@@ -516,7 +517,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L23" activeCellId="0" sqref="L23"/>
     </sheetView>
   </sheetViews>
@@ -679,4 +680,176 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement BCP Automation script for data processing and FTP upload
- Created `bcp_env3.py` to handle client data fetching, processing, and uploading to FTP.
- Added methods for fetching active accounts, client information, contact details, addresses, and dispositions.
- Implemented chunk processing for large datasets to optimize database queries.
- Integrated FTP upload functionality with error handling and directory structure management.
- Enhanced data transformation and mapping using dynamic column mappings from configuration.
- Included logging for process tracking and error reporting.
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SBC CARDS RECOV L1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="FUSE" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="GLOBE WIRELESS" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Info" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="35">
   <si>
     <t xml:space="preserve">Database Column</t>
   </si>
@@ -346,7 +347,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -689,7 +690,7 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -852,4 +853,176 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.65"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>